<commit_message>
Update mainWindow and excelPreview function
</commit_message>
<xml_diff>
--- a/_dane/dane.xlsx
+++ b/_dane/dane.xlsx
@@ -473,35 +473,35 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tak</t>
+          <t>nie</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>89238213</t>
+          <t>696273167</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sasug</t>
+          <t>Samugn</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>dzis</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>opis zleceniea</t>
+          <t xml:space="preserve">opsi	</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">nasze pogu	</t>
+          <t>nas</t>
         </is>
       </c>
     </row>
@@ -512,29 +512,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>34172</v>
+        <v>6</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Note2</t>
+          <t>ddd</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>09/11/2023</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>opis</t>
+          <t xml:space="preserve">oooo	</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>dlans</t>
+          <t>nnnnn</t>
         </is>
       </c>
     </row>
@@ -545,29 +547,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="n">
-        <v>872389173</v>
+        <v>7</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>678 098</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Iphone</t>
+          <t>To ejst mode</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>09/11/2023</t>
+          <t>13/11/2023</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>fajny fest</t>
+          <t>dasddasdjkksdfjsdahfaskfslkfshdjflaflsf	sdkjf</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>kkk</t>
+          <t>ndfmnfnlkjlkjldsjklskjldsfljkdsfljkdfljk</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add names to windows
</commit_message>
<xml_diff>
--- a/_dane/dane.xlsx
+++ b/_dane/dane.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,7 +508,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>nie</t>
+          <t>tak</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -543,7 +543,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>nie</t>
+          <t>tak</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -574,6 +574,56 @@
           <t>ndfmnfnlkjlkjldsjklskjldsfljkdsfljkdfljk</t>
         </is>
       </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>nie</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>dddd</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>16/11/2023</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>nie</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>asdada</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>16/11/2023</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>